<commit_message>
Heaven Gate Editor Stable Version 0.1, Add jump and label function, refactor node stucture
</commit_message>
<xml_diff>
--- a/Documents/Project Manage/Task Check List.xlsx
+++ b/Documents/Project Manage/Task Check List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cookie/Documents/UnityProjectFolder/Hippocampus/Documents/Project Manage/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GithubProjects\Hippocampus\Documents\Project Manage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8493D67-C458-1649-8DE7-1AEACDC4F080}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E10830-0A3B-4F12-9853-CD95C5F7D0B3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="460" windowWidth="28740" windowHeight="16960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist - Task Checklist（S1，S" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="75">
   <si>
     <t>Task Checklist（S1，S2MUST，S3，S4，S5 Should，S6—— Can）</t>
   </si>
@@ -237,6 +237,18 @@
   </si>
   <si>
     <t>Unity，图片资源管理</t>
+  </si>
+  <si>
+    <t>Editor，优化显示，对于不同的类型，制作一个可缩略的选项</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>Editor，增加对于jump和label的提示，禁止死循环</t>
   </si>
 </sst>
 </file>
@@ -244,14 +256,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Avenir Next"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Avenir Next Demi Bold"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -265,8 +284,22 @@
       <name val="Avenir Next Demi Bold"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Avenir Next Demi Bold"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Avenir Next Demi Bold"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,6 +310,28 @@
       <patternFill patternType="solid">
         <fgColor indexed="13"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -479,28 +534,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -515,7 +565,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -524,71 +574,114 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="6" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="6" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="9" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="14" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="13" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="12" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="10" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="11" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
+    <cellStyle name="20% - Accent5" xfId="4" builtinId="46"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1944,31 +2037,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IX57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.1640625" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.140625" defaultRowHeight="21.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="59.33203125" style="1" customWidth="1"/>
-    <col min="4" max="7" width="19.83203125" style="1" customWidth="1"/>
-    <col min="8" max="258" width="8.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="64.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" style="1" customWidth="1"/>
+    <col min="5" max="7" width="19.85546875" style="1" customWidth="1"/>
+    <col min="8" max="258" width="8.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-    </row>
-    <row r="2" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="30" customHeight="1">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+    </row>
+    <row r="2" spans="1:7" ht="22.5" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -1989,946 +2083,973 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A3" s="40" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="5" t="s">
+      <c r="D3" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="21" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="B4" s="7" t="s">
+    <row r="4" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A4" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="8" t="s">
+      <c r="D4" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="23"/>
+      <c r="F4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11" t="s">
+    <row r="5" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A5" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="12" t="s">
+      <c r="E5" s="23"/>
+      <c r="F5" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="B6" s="7" t="s">
+    <row r="6" spans="1:7" ht="36" customHeight="1">
+      <c r="A6" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B6" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="8" t="s">
+      <c r="D6" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="23"/>
+      <c r="F6" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11" t="s">
+    <row r="7" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A7" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="12" t="s">
+      <c r="D7" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="23"/>
+      <c r="F7" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="7" t="s">
+    <row r="8" spans="1:7" ht="30.95" customHeight="1">
+      <c r="A8" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B8" s="25"/>
+      <c r="C8" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="8" t="s">
+      <c r="D8" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="34" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11" t="s">
+    <row r="9" spans="1:7" ht="33.950000000000003" customHeight="1">
+      <c r="A9" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="12" t="s">
+      <c r="D9" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="23"/>
+      <c r="F9" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="7" t="s">
+    <row r="10" spans="1:7" ht="33.75" customHeight="1">
+      <c r="A10" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B10" s="25"/>
+      <c r="C10" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="8" t="s">
+      <c r="D10" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="23"/>
+      <c r="F10" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11" t="s">
+    <row r="11" spans="1:7" ht="33.75" customHeight="1">
+      <c r="A11" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B11" s="25"/>
+      <c r="C11" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="12" t="s">
+      <c r="D11" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="23"/>
+      <c r="F11" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="7" t="s">
+    <row r="12" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A12" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="8" t="s">
+      <c r="D12" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="23"/>
+      <c r="F12" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11" t="s">
+    <row r="13" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A13" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B13" s="25"/>
+      <c r="C13" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="12" t="s">
+      <c r="D13" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="23"/>
+      <c r="F13" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="7" t="s">
+    <row r="14" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A14" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B14" s="25"/>
+      <c r="C14" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="8" t="s">
+      <c r="D14" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="23"/>
+      <c r="F14" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11" t="s">
+    <row r="15" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A15" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B15" s="25"/>
+      <c r="C15" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="12" t="s">
+      <c r="D15" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="23"/>
+      <c r="F15" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G15" s="24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="7" t="s">
+    <row r="16" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A16" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B16" s="25"/>
+      <c r="C16" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="29" t="s">
+      <c r="D16" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="23"/>
+      <c r="F16" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11" t="s">
+    <row r="17" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A17" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="30" t="s">
+      <c r="D17" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="28" t="s">
+      <c r="G17" s="31" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="7" t="s">
+    <row r="18" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A18" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B18" s="27"/>
+      <c r="C18" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="30" t="s">
+      <c r="D18" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="F18" s="27" t="s">
+      <c r="F18" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="30" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="11" t="s">
+    <row r="19" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A19" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B19" s="27"/>
+      <c r="C19" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="31" t="s">
+      <c r="D19" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G19" s="30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="7" t="s">
+    <row r="20" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A20" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B20" s="27"/>
+      <c r="C20" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="30" t="s">
+      <c r="D20" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="11" t="s">
+    <row r="21" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A21" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B21" s="27"/>
+      <c r="C21" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="31" t="s">
+      <c r="D21" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G21" s="30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="7" t="s">
+    <row r="22" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A22" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B22" s="27"/>
+      <c r="C22" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="30" t="s">
+      <c r="D22" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="30" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="11" t="s">
+    <row r="23" spans="1:7" ht="21.95" customHeight="1">
+      <c r="A23" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="31" t="s">
+      <c r="D23" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G23" s="12" t="s">
+      <c r="G23" s="30" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="11" t="s">
+    <row r="24" spans="1:7" ht="24" customHeight="1">
+      <c r="A24" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B24" s="27"/>
+      <c r="C24" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="30" t="s">
+      <c r="D24" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="F24" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="G24" s="30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="7" t="s">
+    <row r="25" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A25" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B25" s="27"/>
+      <c r="C25" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="30" t="s">
+      <c r="D25" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F25" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G25" s="8" t="s">
+      <c r="G25" s="30" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="8"/>
-    </row>
-    <row r="27" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C27" s="18" t="s">
+    <row r="26" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A26" s="41"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="33"/>
+    </row>
+    <row r="27" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A27" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B27" s="33"/>
+      <c r="C27" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="30" t="s">
+      <c r="D27" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="12" t="s">
+      <c r="G27" s="30" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="11" t="s">
+    <row r="28" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A28" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="C28" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" s="31" t="s">
+      <c r="D28" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F28" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G28" s="12" t="s">
+      <c r="G28" s="30" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="7" t="s">
+    <row r="29" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A29" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="30" t="s">
+      <c r="D29" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="F29" s="12" t="s">
+      <c r="F29" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G29" s="8" t="s">
+      <c r="G29" s="30" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18" t="s">
+    <row r="30" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A30" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="D30" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="31" t="s">
+      <c r="D30" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G30" s="8" t="s">
+      <c r="G30" s="30" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="8"/>
-    </row>
-    <row r="32" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18" t="s">
+    <row r="31" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A31" s="41"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="33"/>
+    </row>
+    <row r="32" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A32" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B32" s="34"/>
+      <c r="C32" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" s="30" t="s">
+      <c r="D32" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="F32" s="12" t="s">
+      <c r="F32" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G32" s="12" t="s">
+      <c r="G32" s="30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23" t="s">
+    <row r="33" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A33" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B33" s="35"/>
+      <c r="C33" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" s="32" t="s">
+      <c r="D33" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="F33" s="19" t="s">
+      <c r="F33" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="G33" s="20" t="s">
+      <c r="G33" s="37" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23" t="s">
+    <row r="34" spans="1:7" ht="22.7" customHeight="1">
+      <c r="A34" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="B34" s="35"/>
+      <c r="C34" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="D34" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" s="33" t="s">
+      <c r="D34" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="F34" s="19"/>
-      <c r="G34" s="20" t="s">
+      <c r="F34" s="36"/>
+      <c r="G34" s="37" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="20"/>
-    </row>
-    <row r="36" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="25"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="20"/>
-    </row>
-    <row r="37" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B37" s="13"/>
-      <c r="C37" s="7" t="s">
+    <row r="35" spans="1:7" ht="22.5" customHeight="1">
+      <c r="A35" s="42"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="37"/>
+    </row>
+    <row r="36" spans="1:7" ht="22.5" customHeight="1">
+      <c r="A36" s="42"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="37"/>
+    </row>
+    <row r="37" spans="1:7" ht="22.5" customHeight="1">
+      <c r="A37" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="B37" s="17"/>
+      <c r="C37" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="21" t="s">
+      <c r="D37" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F37" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G37" s="24" t="s">
+      <c r="G37" s="18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="B38" s="13"/>
-      <c r="C38" s="7" t="s">
+    <row r="38" spans="1:7" ht="22.5" customHeight="1">
+      <c r="A38" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B38" s="27"/>
+      <c r="C38" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" s="24" t="s">
+      <c r="D38" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="F38" s="12" t="s">
+      <c r="F38" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G38" s="24" t="s">
+      <c r="G38" s="39" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="B39" s="10"/>
-      <c r="C39" s="11" t="s">
+    <row r="39" spans="1:7" ht="22.5" customHeight="1">
+      <c r="A39" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B39" s="27"/>
+      <c r="C39" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="24" t="s">
+      <c r="D39" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F39" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G39" s="24" t="s">
+      <c r="G39" s="39" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B40" s="16"/>
-      <c r="C40" s="8" t="s">
+    <row r="40" spans="1:7" ht="22.5" customHeight="1">
+      <c r="A40" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B40" s="29"/>
+      <c r="C40" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="D40" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" s="24" t="s">
+      <c r="D40" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="F40" s="8" t="s">
+      <c r="F40" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G40" s="24" t="s">
+      <c r="G40" s="39" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B41" s="23"/>
-      <c r="C41" s="23" t="s">
+    <row r="41" spans="1:7" ht="22.5" customHeight="1">
+      <c r="A41" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B41" s="35"/>
+      <c r="C41" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="D41" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="24" t="s">
+      <c r="D41" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="F41" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G41" s="24" t="s">
+      <c r="G41" s="39" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="B42" s="23"/>
-      <c r="C42" s="23" t="s">
+    <row r="42" spans="1:7" ht="22.5" customHeight="1">
+      <c r="A42" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B42" s="35"/>
+      <c r="C42" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="D42" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" s="24" t="s">
+      <c r="D42" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="F42" s="12" t="s">
+      <c r="F42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G42" s="24" t="s">
+      <c r="G42" s="39" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="B43" s="23"/>
-      <c r="C43" s="23" t="s">
+    <row r="43" spans="1:7" ht="22.5" customHeight="1">
+      <c r="A43" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="B43" s="35"/>
+      <c r="C43" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="D43" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" s="24" t="s">
+      <c r="D43" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="F43" s="8" t="s">
+      <c r="F43" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G43" s="24" t="s">
+      <c r="G43" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="B44" s="23"/>
-      <c r="C44" s="23" t="s">
+    <row r="44" spans="1:7" ht="22.5" customHeight="1">
+      <c r="A44" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="B44" s="35"/>
+      <c r="C44" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="D44" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" s="24" t="s">
+      <c r="D44" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="F44" s="8" t="s">
+      <c r="F44" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G44" s="24" t="s">
+      <c r="G44" s="39" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="25"/>
-      <c r="B45" s="23"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
-    </row>
-    <row r="46" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="25"/>
-      <c r="B46" s="23"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24"/>
-      <c r="G46" s="24"/>
-    </row>
-    <row r="47" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="25"/>
-      <c r="B47" s="23"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="24"/>
-      <c r="G47" s="24"/>
-    </row>
-    <row r="48" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="22" t="s">
+    <row r="45" spans="1:7" ht="22.5" customHeight="1">
+      <c r="A45" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="B45" s="35"/>
+      <c r="C45" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="D45" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="F45" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="G45" s="39" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="22.5" customHeight="1">
+      <c r="A46" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="B46" s="35"/>
+      <c r="C46" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="D46" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="F46" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="G46" s="39" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="22.5" customHeight="1">
+      <c r="A47" s="42"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="39"/>
+    </row>
+    <row r="48" spans="1:7" ht="21.75" customHeight="1">
+      <c r="A48" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="22"/>
-      <c r="C48" s="22"/>
-      <c r="D48" s="22"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="22"/>
-      <c r="G48" s="22"/>
-    </row>
-    <row r="49" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B49" s="10"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="17"/>
-      <c r="G49" s="12"/>
-    </row>
-    <row r="50" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="B50" s="13"/>
-      <c r="C50" s="7" t="s">
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+    </row>
+    <row r="49" spans="1:7" ht="21.75" customHeight="1">
+      <c r="A49" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="B49" s="7"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="9"/>
+    </row>
+    <row r="50" spans="1:7" ht="21.75" customHeight="1">
+      <c r="A50" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B50" s="10"/>
+      <c r="C50" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E50" s="16"/>
-      <c r="F50" s="8" t="s">
+      <c r="E50" s="11"/>
+      <c r="F50" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="8" t="s">
+      <c r="G50" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B51" s="10"/>
-      <c r="C51" s="11" t="s">
+    <row r="51" spans="1:7" ht="21.75" customHeight="1">
+      <c r="A51" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="B51" s="7"/>
+      <c r="C51" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D51" s="11" t="s">
+      <c r="D51" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E51" s="17"/>
-      <c r="F51" s="12" t="s">
+      <c r="E51" s="12"/>
+      <c r="F51" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G51" s="12" t="s">
+      <c r="G51" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="B52" s="13"/>
-      <c r="C52" s="7" t="s">
+    <row r="52" spans="1:7" ht="21.75" customHeight="1">
+      <c r="A52" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B52" s="10"/>
+      <c r="C52" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E52" s="16"/>
-      <c r="F52" s="8" t="s">
+      <c r="E52" s="11"/>
+      <c r="F52" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G52" s="8" t="s">
+      <c r="G52" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="14" t="s">
+    <row r="56" spans="1:7" ht="21.75" customHeight="1">
+      <c r="A56" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-    </row>
-    <row r="57" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B57" s="10"/>
-      <c r="C57" s="11" t="s">
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+    </row>
+    <row r="57" spans="1:7" ht="21.75" customHeight="1">
+      <c r="A57" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="B57" s="7"/>
+      <c r="C57" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D57" s="11" t="s">
+      <c r="D57" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E57" s="17"/>
-      <c r="F57" s="12" t="s">
+      <c r="E57" s="12"/>
+      <c r="F57" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G57" s="12" t="s">
+      <c r="G57" s="9" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor story window framework
</commit_message>
<xml_diff>
--- a/Documents/Project Manage/Task Check List.xlsx
+++ b/Documents/Project Manage/Task Check List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GithubProjects\Hippocampus\Documents\Project Manage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84F45A2-BE7D-4C94-A82B-79262AA5D3D8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEC8970-E19F-46D7-AFAC-D59E539ED878}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="81">
   <si>
     <t>Date</t>
   </si>
@@ -257,6 +257,24 @@
   </si>
   <si>
     <t>P5</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>All Task Estimated Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> All time we have</t>
   </si>
 </sst>
 </file>
@@ -266,12 +284,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Avenir Next"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Avenir Next Demi Bold"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -334,6 +359,13 @@
       <name val="Avenir Next Demi Bold"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Avenir Next"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="7">
@@ -575,19 +607,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -620,139 +652,151 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="6" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="6" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="9" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="7" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="6" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="6" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="9" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="7" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="12" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="10" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="12" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="10" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="6" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="6" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="6" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2116,8 +2160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IX61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.140625" defaultRowHeight="21.75" customHeight="1"/>
@@ -2132,15 +2176,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
     </row>
     <row r="2" spans="1:8" ht="22.5" customHeight="1">
       <c r="A2" s="2"/>
@@ -2443,7 +2487,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="25"/>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="58" t="s">
         <v>48</v>
       </c>
       <c r="D17" s="26" t="s">
@@ -2471,16 +2515,16 @@
       <c r="D18" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="55" t="s">
+      <c r="E18" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="56" t="s">
+      <c r="F18" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="57">
+      <c r="G18" s="55">
         <v>4</v>
       </c>
-      <c r="H18" s="57">
+      <c r="H18" s="55">
         <v>6</v>
       </c>
     </row>
@@ -2533,7 +2577,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="25"/>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="58" t="s">
         <v>41</v>
       </c>
       <c r="D21" s="26" t="s">
@@ -2555,7 +2599,7 @@
         <v>0</v>
       </c>
       <c r="B22" s="25"/>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="58" t="s">
         <v>42</v>
       </c>
       <c r="D22" s="26" t="s">
@@ -2599,7 +2643,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="25"/>
-      <c r="C24" s="54" t="s">
+      <c r="C24" s="52" t="s">
         <v>30</v>
       </c>
       <c r="D24" s="26" t="s">
@@ -2621,7 +2665,7 @@
         <v>0</v>
       </c>
       <c r="B25" s="25"/>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="58" t="s">
         <v>47</v>
       </c>
       <c r="D25" s="26" t="s">
@@ -2751,7 +2795,7 @@
         <v>0</v>
       </c>
       <c r="B32" s="30"/>
-      <c r="C32" s="30" t="s">
+      <c r="C32" s="59" t="s">
         <v>45</v>
       </c>
       <c r="D32" s="26" t="s">
@@ -2815,13 +2859,13 @@
         <v>0</v>
       </c>
       <c r="B35" s="31"/>
-      <c r="C35" s="52" t="s">
+      <c r="C35" s="50" t="s">
         <v>73</v>
       </c>
       <c r="D35" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E35" s="53" t="s">
+      <c r="E35" s="51" t="s">
         <v>74</v>
       </c>
       <c r="F35" s="32"/>
@@ -3090,10 +3134,16 @@
       <c r="C48" s="40"/>
       <c r="D48" s="31"/>
       <c r="E48" s="34"/>
-      <c r="F48" s="34"/>
+      <c r="F48" s="61" t="s">
+        <v>79</v>
+      </c>
       <c r="G48" s="49">
         <f>SUM(G17:G47)</f>
         <v>130</v>
+      </c>
+      <c r="H48" s="60">
+        <f>SUM(H18:H47)</f>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="22.5" customHeight="1">
@@ -3102,7 +3152,9 @@
       <c r="C49" s="40"/>
       <c r="D49" s="31"/>
       <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
+      <c r="F49" s="61" t="s">
+        <v>80</v>
+      </c>
       <c r="G49" s="41" t="s">
         <v>71</v>
       </c>
@@ -3126,15 +3178,15 @@
       <c r="G51" s="34"/>
     </row>
     <row r="52" spans="1:7" ht="21.75" customHeight="1">
-      <c r="A52" s="51" t="s">
+      <c r="A52" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="B52" s="51"/>
-      <c r="C52" s="51"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="51"/>
-      <c r="F52" s="51"/>
-      <c r="G52" s="51"/>
+      <c r="B52" s="57"/>
+      <c r="C52" s="57"/>
+      <c r="D52" s="57"/>
+      <c r="E52" s="57"/>
+      <c r="F52" s="57"/>
+      <c r="G52" s="57"/>
     </row>
     <row r="53" spans="1:7" ht="21.75" customHeight="1">
       <c r="A53" s="6" t="b">
@@ -3205,15 +3257,15 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="21.75" customHeight="1">
-      <c r="A60" s="50" t="s">
+      <c r="A60" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="B60" s="50"/>
-      <c r="C60" s="50"/>
-      <c r="D60" s="50"/>
-      <c r="E60" s="50"/>
-      <c r="F60" s="50"/>
-      <c r="G60" s="50"/>
+      <c r="B60" s="56"/>
+      <c r="C60" s="56"/>
+      <c r="D60" s="56"/>
+      <c r="E60" s="56"/>
+      <c r="F60" s="56"/>
+      <c r="G60" s="56"/>
     </row>
     <row r="61" spans="1:7" ht="21.75" customHeight="1">
       <c r="A61" s="6" t="b">

</xml_diff>